<commit_message>
Adding new updated API error file
Adding new updated API error consolidated List 4-22-25
</commit_message>
<xml_diff>
--- a/Error Inventory/API Error Consolidated List.xlsx
+++ b/Error Inventory/API Error Consolidated List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eagnmnwbp130a.usa.dce.usps.gov\VDIProfiles$\fsbtg0\Documents\API Consolidated file to upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A437FC1D-9988-48D8-B5D3-B8B52B49C195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A151C24B-DDC8-470E-BAE3-97FFE4821CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14040" firstSheet="4" activeTab="4" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
   </bookViews>
@@ -24,10 +24,11 @@
     <sheet name="International Prices" sheetId="7" r:id="rId9"/>
     <sheet name="Location" sheetId="13" r:id="rId10"/>
     <sheet name="Payment" sheetId="18" r:id="rId11"/>
-    <sheet name="Scan Form" sheetId="14" r:id="rId12"/>
-    <sheet name="Service Standards" sheetId="17" r:id="rId13"/>
-    <sheet name="Shipping Options" sheetId="16" r:id="rId14"/>
-    <sheet name="Tracking" sheetId="1" r:id="rId15"/>
+    <sheet name="PMOD(Open and Distribute)" sheetId="19" r:id="rId12"/>
+    <sheet name="Scan Form" sheetId="14" r:id="rId13"/>
+    <sheet name="Service Standards" sheetId="17" r:id="rId14"/>
+    <sheet name="Shipping Options" sheetId="16" r:id="rId15"/>
+    <sheet name="Tracking" sheetId="1" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Addresses!$A$1:$G$3</definedName>
@@ -36,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Domestic Prices'!$A$1:$G$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'General Errors'!$A$1:$D$82</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'International Prices'!$A$1:$G$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Tracking!$A$1:$G$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Tracking!$A$1:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3547" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3678" uniqueCount="931">
   <si>
     <t>API</t>
   </si>
@@ -2755,12 +2756,6 @@
     <t>customer reference #3 cannot be used with a customs form</t>
   </si>
   <si>
-    <t>16316</t>
-  </si>
-  <si>
-    <t>16317</t>
-  </si>
-  <si>
     <t>indiciaDescription.mailClass, indiciaDescription.extraServices</t>
   </si>
   <si>
@@ -2774,6 +2769,101 @@
   </si>
   <si>
     <t>https://api.usps.com/labels/v3/indicia</t>
+  </si>
+  <si>
+    <t>imageInfo.brandingImageUUIDs</t>
+  </si>
+  <si>
+    <t>imageInfo.brandingImageFormat</t>
+  </si>
+  <si>
+    <t>brandingImageUUIDs must contain only two UUIDs when brandingImageFormat is 'TWO_SQUARES'</t>
+  </si>
+  <si>
+    <t>brandingImageUUIDs must contain only one UUID when brandingImageFormat is 'ONE_SQUARE' or 'RECTANGLE'</t>
+  </si>
+  <si>
+    <t>brandingImageFormat is required when brandingImageUUIDs are provided</t>
+  </si>
+  <si>
+    <t>customer reference #3-4 cannot be used with a branding image</t>
+  </si>
+  <si>
+    <t>brandingImageFormat currently does not support imageInfo.imageType of 'ZPL203DPI' or 'ZPL300DPI'</t>
+  </si>
+  <si>
+    <t>PMOD</t>
+  </si>
+  <si>
+    <t>https://api.usps.com/pmod/v3/pmod/create</t>
+  </si>
+  <si>
+    <t>destinationEntryFacilityType must be 'DESTINATION_DELIVERY_UNIT' or 'DESTINATION_SERVICE_HUB' when processingCategory is 'MIXED'</t>
+  </si>
+  <si>
+    <t>Max image count 50 reached. Unable to upload. Images may be deleted to free space.</t>
+  </si>
+  <si>
+    <t>Crid provided in request was malformed</t>
+  </si>
+  <si>
+    <t>Invalid image provided. Image must be a valid SVG element base64 encoded.</t>
+  </si>
+  <si>
+    <t>Image with provided CRID + imageUUID does not exist for deletion</t>
+  </si>
+  <si>
+    <t>Image with provided CRID + imageUUID does not exist for retrieval</t>
+  </si>
+  <si>
+    <t>imageinfo.imagedata</t>
+  </si>
+  <si>
+    <t>The svg must contain a viewbox or length + width attributes</t>
+  </si>
+  <si>
+    <t>https://api.usps.com/labels/v3/branding</t>
+  </si>
+  <si>
+    <t>https://api.usps.com/labels/v3/branding/{imageUUID}</t>
+  </si>
+  <si>
+    <t>imageUUID
+CRID</t>
+  </si>
+  <si>
+    <t>CRID</t>
+  </si>
+  <si>
+    <t>provided brandingImageUUID does not exist</t>
+  </si>
+  <si>
+    <t>imageUUID</t>
+  </si>
+  <si>
+    <t>When 931 or 934 service codes are present, item value must be greater than 500</t>
+  </si>
+  <si>
+    <t>No locker is available for your size package</t>
+  </si>
+  <si>
+    <t>Address supplied is not a deliverable address: R777 Phantom Route physical address is not deliverable. Contact the recipient for their USPS Mail delivery address.</t>
+  </si>
+  <si>
+    <t>SVG element type 'image' with attribute 'xlink:href' is forbidden</t>
+  </si>
+  <si>
+    <t>SVG element type `script` is forbidden</t>
+  </si>
+  <si>
+    <t>SVG element type `style` is forbidden</t>
+  </si>
+  <si>
+    <t>SVG element type 'use' with attribute 'xlink:href' is forbidden</t>
+  </si>
+  <si>
+    <t>https://api.usps.com/pmod/v3/pmod/create
+https://api.usps.com/pmod/v3/pmod/manifest/{container-id}</t>
   </si>
 </sst>
 </file>
@@ -3015,7 +3105,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4149,6 +4241,157 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C1B7C1-6FF6-49B7-8FF7-3B1E3D2E2BE9}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="126" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B2" s="10">
+        <v>400</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>873</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B3" s="10">
+        <v>400</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E3" s="24">
+        <v>160299</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>875</v>
+      </c>
+      <c r="G3" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B4" s="10">
+        <v>400</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>908</v>
+      </c>
+      <c r="E4" s="17">
+        <v>160321</v>
+      </c>
+      <c r="F4" t="s">
+        <v>876</v>
+      </c>
+      <c r="G4" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B5" s="10">
+        <v>400</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>930</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>830</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080706B6-9387-41AC-AEC7-FBA9784CBC33}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -4541,7 +4784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E19D90B-8A7E-4C9D-8766-50872932F6BA}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -4660,7 +4903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6B6B6E-42EB-430D-822F-B7D19114F059}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5528,7 +5771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3BB263-4572-4BC8-8AF5-D80D70E936F3}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -5862,7 +6105,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6088,7 +6331,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6581,8 +6824,8 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6974,11 +7217,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E189" sqref="E189"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11203,17 +11446,17 @@
       <c r="C184" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D184" s="45" t="s">
-        <v>901</v>
-      </c>
-      <c r="E184" s="17" t="s">
+      <c r="D184" t="s">
+        <v>899</v>
+      </c>
+      <c r="E184" s="17">
+        <v>160316</v>
+      </c>
+      <c r="F184" s="33" t="s">
         <v>895</v>
       </c>
-      <c r="F184" s="33" t="s">
+      <c r="G184" s="2" t="s">
         <v>897</v>
-      </c>
-      <c r="G184" s="2" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -11226,17 +11469,475 @@
       <c r="C185" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D185" s="45" t="s">
+      <c r="D185" t="s">
+        <v>899</v>
+      </c>
+      <c r="E185" s="17">
+        <v>160317</v>
+      </c>
+      <c r="F185" s="33" t="s">
+        <v>896</v>
+      </c>
+      <c r="G185" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B186" s="20">
+        <v>400</v>
+      </c>
+      <c r="C186" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D186" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E186" s="17">
+        <v>160326</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="G186" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B187" s="20">
+        <v>400</v>
+      </c>
+      <c r="C187" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D187" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E187" s="17">
+        <v>160327</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="G187" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B188" s="20">
+        <v>400</v>
+      </c>
+      <c r="C188" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D188" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E188" s="17">
+        <v>160328</v>
+      </c>
+      <c r="F188" s="2" t="s">
         <v>901</v>
       </c>
-      <c r="E185" s="17" t="s">
+      <c r="G188" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B189" s="20">
+        <v>400</v>
+      </c>
+      <c r="C189" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D189" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E189" s="17">
+        <v>160329</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="G189" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B190" s="20">
+        <v>400</v>
+      </c>
+      <c r="C190" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D190" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E190" s="17">
+        <v>160330</v>
+      </c>
+      <c r="F190" s="37" t="s">
+        <v>715</v>
+      </c>
+      <c r="G190" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B191" s="20">
+        <v>400</v>
+      </c>
+      <c r="C191" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D191" t="s">
+        <v>92</v>
+      </c>
+      <c r="E191" s="17">
+        <v>160336</v>
+      </c>
+      <c r="F191" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="G191" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B192" s="20">
+        <v>400</v>
+      </c>
+      <c r="C192" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D192" t="s">
+        <v>917</v>
+      </c>
+      <c r="E192" s="17">
+        <v>160331</v>
+      </c>
+      <c r="F192" s="37"/>
+      <c r="G192" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B193" s="20">
+        <v>400</v>
+      </c>
+      <c r="C193" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D193" t="s">
+        <v>917</v>
+      </c>
+      <c r="E193" s="17">
+        <v>160332</v>
+      </c>
+      <c r="F193" s="37" t="s">
+        <v>920</v>
+      </c>
+      <c r="G193" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B194" s="20">
+        <v>400</v>
+      </c>
+      <c r="C194" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D194" t="s">
+        <v>917</v>
+      </c>
+      <c r="E194" s="17">
+        <v>160333</v>
+      </c>
+      <c r="F194" s="17" t="s">
+        <v>915</v>
+      </c>
+      <c r="G194" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B195" s="21">
+        <v>400</v>
+      </c>
+      <c r="C195" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>918</v>
+      </c>
+      <c r="E195" s="24">
+        <v>160334</v>
+      </c>
+      <c r="F195" s="37" t="s">
+        <v>919</v>
+      </c>
+      <c r="G195" s="10" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B196" s="21">
+        <v>400</v>
+      </c>
+      <c r="C196" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D196" s="10" t="s">
+        <v>918</v>
+      </c>
+      <c r="E196" s="24">
+        <v>160335</v>
+      </c>
+      <c r="F196" s="37" t="s">
+        <v>919</v>
+      </c>
+      <c r="G196" s="10" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B197" s="21">
+        <v>400</v>
+      </c>
+      <c r="C197" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D197" t="s">
+        <v>917</v>
+      </c>
+      <c r="E197" s="17">
+        <v>160337</v>
+      </c>
+      <c r="F197" s="17" t="s">
+        <v>915</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B198" s="21">
+        <v>400</v>
+      </c>
+      <c r="C198" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D198" t="s">
+        <v>918</v>
+      </c>
+      <c r="E198" s="17">
+        <v>160338</v>
+      </c>
+      <c r="F198" s="37" t="s">
+        <v>922</v>
+      </c>
+      <c r="G198" s="2" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B199" s="21">
+        <v>400</v>
+      </c>
+      <c r="C199" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D199" t="s">
+        <v>899</v>
+      </c>
+      <c r="E199" s="17">
+        <v>160322</v>
+      </c>
+      <c r="F199" t="s">
         <v>896</v>
       </c>
-      <c r="F185" s="33" t="s">
-        <v>898</v>
-      </c>
-      <c r="G185" s="2" t="s">
-        <v>900</v>
+      <c r="G199" s="2" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B200" s="21">
+        <v>400</v>
+      </c>
+      <c r="C200" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D200" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E200" s="17">
+        <v>160319</v>
+      </c>
+      <c r="F200" t="s">
+        <v>719</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B201" s="21">
+        <v>400</v>
+      </c>
+      <c r="C201" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D201" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E201" s="24">
+        <v>160320</v>
+      </c>
+      <c r="F201" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B202" s="20">
+        <v>400</v>
+      </c>
+      <c r="C202" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D202" t="s">
+        <v>917</v>
+      </c>
+      <c r="E202" s="24">
+        <v>160339</v>
+      </c>
+      <c r="F202" s="17" t="s">
+        <v>915</v>
+      </c>
+      <c r="G202" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B203" s="20">
+        <v>400</v>
+      </c>
+      <c r="C203" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D203" t="s">
+        <v>917</v>
+      </c>
+      <c r="E203" s="24">
+        <v>160340</v>
+      </c>
+      <c r="F203" s="17" t="s">
+        <v>915</v>
+      </c>
+      <c r="G203" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B204" s="20">
+        <v>400</v>
+      </c>
+      <c r="C204" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D204" t="s">
+        <v>917</v>
+      </c>
+      <c r="E204" s="24">
+        <v>160341</v>
+      </c>
+      <c r="F204" s="17" t="s">
+        <v>915</v>
+      </c>
+      <c r="G204" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B205" s="20">
+        <v>400</v>
+      </c>
+      <c r="C205" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D205" t="s">
+        <v>917</v>
+      </c>
+      <c r="E205" s="24">
+        <v>160342</v>
+      </c>
+      <c r="F205" s="17" t="s">
+        <v>915</v>
+      </c>
+      <c r="G205" t="s">
+        <v>929</v>
       </c>
     </row>
   </sheetData>
@@ -11252,10 +11953,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="D171" workbookViewId="0">
+      <selection activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15366,6 +16067,29 @@
       </c>
       <c r="G180" s="2" t="s">
         <v>710</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B181" s="21">
+        <v>400</v>
+      </c>
+      <c r="C181" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D181" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E181" s="24">
+        <v>160320</v>
+      </c>
+      <c r="F181" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="G181" s="2" t="s">
+        <v>925</v>
       </c>
     </row>
   </sheetData>
@@ -16290,9 +17014,9 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17139,7 +17863,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17810,19 +18534,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -17831,7 +18542,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD1EFD7F07544F4C8A5DF6ACE5557D0F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0a46465e297c47d8b88a71685f887e65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9" xmlns:ns3="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4503a5f252426d71f93d44927b16e869" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18077,25 +18788,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DC8D4E-C199-4BF9-AF5D-F16C7D7041E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -18103,7 +18809,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11AB0D6-FBA0-4F11-8778-05A9ADBB93A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18123,6 +18829,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DC8D4E-C199-4BF9-AF5D-F16C7D7041E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6c9b68e5-0371-4f27-93af-8d15f794dc29}" enabled="1" method="Privileged" siteId="{a01f407a-85cb-4a16-98bb-f28e6384bd28}" removed="0"/>

</xml_diff>

<commit_message>
Update to the existing API example file
Update to the existing API example file to match the deployment changes
</commit_message>
<xml_diff>
--- a/Error Inventory/API Error Consolidated List.xlsx
+++ b/Error Inventory/API Error Consolidated List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eagnmnwbp130a.usa.dce.usps.gov\VDIProfiles$\fsbtg0\Documents\API Consolidated file to upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A151C24B-DDC8-470E-BAE3-97FFE4821CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B525B85-05F7-41C5-828E-6FF531CAF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14040" firstSheet="4" activeTab="4" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3678" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3758" uniqueCount="946">
   <si>
     <t>API</t>
   </si>
@@ -2864,6 +2864,51 @@
   <si>
     <t>https://api.usps.com/pmod/v3/pmod/create
 https://api.usps.com/pmod/v3/pmod/manifest/{container-id}</t>
+  </si>
+  <si>
+    <t>Container does not have any packages associated with it</t>
+  </si>
+  <si>
+    <t>Container is not a PMOD container</t>
+  </si>
+  <si>
+    <t>Unable to find valid label with trackingNumber: &lt;trackingNumber&gt;</t>
+  </si>
+  <si>
+    <t>Unable to add Priority Mail Express label &lt;barcode&gt; to Priority Mail Express Open Distribute container</t>
+  </si>
+  <si>
+    <t>Unable to add hazmat label &lt;barcode&gt; to Priority Mail Express Open Distribute container</t>
+  </si>
+  <si>
+    <t>Label &lt;barcode&gt; with status &lt;status&gt; is unable to be added to container</t>
+  </si>
+  <si>
+    <t>Unable to add label &lt;barcode&gt; with mail class &lt;mailClass&gt; to Open Distribute Container</t>
+  </si>
+  <si>
+    <t>trackingNumbers</t>
+  </si>
+  <si>
+    <t>containerId</t>
+  </si>
+  <si>
+    <t>https://api.usps.com/pmod/v3/pmod/manifest/{container-id}</t>
+  </si>
+  <si>
+    <t>4X4LABEL is not supported for this request</t>
+  </si>
+  <si>
+    <t>TWO_SQUARES' is supported on the following 'imageInfo.labelType' values: ['4X6LABEL', '4X5LABEL']</t>
+  </si>
+  <si>
+    <t>ONE_SQUARE' is supported on the following 'imageInfo.labelType' values: ['4X6LABEL', '4X5LABEL', and '2X7LABEL']</t>
+  </si>
+  <si>
+    <t>RECTANGLE' is supported on the following 'imageInfo.labelType' values: ['4X6LABEL', '4X5LABEL']</t>
+  </si>
+  <si>
+    <t>RECTANGLE' is only supported for Return Labels with 'imageInfo.labelType' of '4X5LABEL'</t>
   </si>
 </sst>
 </file>
@@ -2975,7 +3020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3104,9 +3149,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4245,10 +4287,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4364,7 +4406,7 @@
       <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="2" t="s">
         <v>930</v>
       </c>
       <c r="E5" s="24" t="s">
@@ -4377,14 +4419,166 @@
         <v>216</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B6" s="10">
+        <v>400</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>940</v>
+      </c>
+      <c r="E6" s="17">
+        <v>160344</v>
+      </c>
+      <c r="F6" t="s">
+        <v>939</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>931</v>
+      </c>
+    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="24"/>
+      <c r="A7" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B7" s="10">
+        <v>400</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>940</v>
+      </c>
+      <c r="E7" s="17">
+        <v>160345</v>
+      </c>
+      <c r="F7" t="s">
+        <v>939</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="24"/>
+      <c r="A8" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B8" s="10">
+        <v>400</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E8" s="17">
+        <v>160350</v>
+      </c>
+      <c r="F8" t="s">
+        <v>938</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>933</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="17"/>
+      <c r="A9" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B9" s="10">
+        <v>400</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E9" s="17">
+        <v>160352</v>
+      </c>
+      <c r="F9" t="s">
+        <v>938</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B10" s="10">
+        <v>400</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E10" s="17">
+        <v>160353</v>
+      </c>
+      <c r="F10" t="s">
+        <v>938</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B11" s="10">
+        <v>400</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E11" s="17">
+        <v>160354</v>
+      </c>
+      <c r="F11" t="s">
+        <v>938</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B12" s="10">
+        <v>400</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E12" s="17">
+        <v>160355</v>
+      </c>
+      <c r="F12" t="s">
+        <v>938</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>937</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7217,11 +7411,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G205"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D208" sqref="D208"/>
+      <selection pane="bottomLeft" activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11940,6 +12134,98 @@
         <v>929</v>
       </c>
     </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B206" s="20">
+        <v>400</v>
+      </c>
+      <c r="C206" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D206" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E206" s="17">
+        <v>160347</v>
+      </c>
+      <c r="F206" s="37" t="s">
+        <v>901</v>
+      </c>
+      <c r="G206" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B207" s="20">
+        <v>400</v>
+      </c>
+      <c r="C207" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D207" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E207" s="17">
+        <v>160348</v>
+      </c>
+      <c r="F207" s="37" t="s">
+        <v>901</v>
+      </c>
+      <c r="G207" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B208" s="20">
+        <v>400</v>
+      </c>
+      <c r="C208" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D208" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E208" s="17">
+        <v>160349</v>
+      </c>
+      <c r="F208" s="37" t="s">
+        <v>901</v>
+      </c>
+      <c r="G208" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B209" s="20">
+        <v>400</v>
+      </c>
+      <c r="C209" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D209" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E209" s="17">
+        <v>160351</v>
+      </c>
+      <c r="F209" s="37" t="s">
+        <v>901</v>
+      </c>
+      <c r="G209" t="s">
+        <v>945</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{A36F69E6-5AC8-443F-8567-4E3FB7E927F1}"/>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -11953,10 +12239,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G186"/>
   <sheetViews>
     <sheetView topLeftCell="D171" workbookViewId="0">
-      <selection activeCell="E184" sqref="E184"/>
+      <selection activeCell="E183" sqref="E183:G186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16090,6 +16376,121 @@
       </c>
       <c r="G181" s="2" t="s">
         <v>925</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B182" s="21">
+        <v>400</v>
+      </c>
+      <c r="C182" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D182" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E182" s="17">
+        <v>160346</v>
+      </c>
+      <c r="F182" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="G182" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B183" s="21">
+        <v>400</v>
+      </c>
+      <c r="C183" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D183" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E183" s="17">
+        <v>160347</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="G183" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B184" s="21">
+        <v>400</v>
+      </c>
+      <c r="C184" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D184" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E184" s="17">
+        <v>160348</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="G184" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B185" s="21">
+        <v>400</v>
+      </c>
+      <c r="C185" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E185" s="17">
+        <v>160349</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="G185" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B186" s="21">
+        <v>400</v>
+      </c>
+      <c r="C186" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D186" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E186" s="17">
+        <v>160351</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="G186" t="s">
+        <v>945</v>
       </c>
     </row>
   </sheetData>
@@ -18534,6 +18935,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -18542,7 +18956,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD1EFD7F07544F4C8A5DF6ACE5557D0F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0a46465e297c47d8b88a71685f887e65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9" xmlns:ns3="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4503a5f252426d71f93d44927b16e869" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18788,20 +19202,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DC8D4E-C199-4BF9-AF5D-F16C7D7041E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -18809,7 +19228,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11AB0D6-FBA0-4F11-8778-05A9ADBB93A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18829,24 +19248,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DC8D4E-C199-4BF9-AF5D-F16C7D7041E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6c9b68e5-0371-4f27-93af-8d15f794dc29}" enabled="1" method="Privileged" siteId="{a01f407a-85cb-4a16-98bb-f28e6384bd28}" removed="0"/>

</xml_diff>

<commit_message>
Updating file for May 28 release
API Error file updates for May 28 Release
</commit_message>
<xml_diff>
--- a/Error Inventory/API Error Consolidated List.xlsx
+++ b/Error Inventory/API Error Consolidated List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eagnmnwbp130a.usa.dce.usps.gov\VDIProfiles$\fsbtg0\Documents\API Consolidated file to upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B525B85-05F7-41C5-828E-6FF531CAF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51CC7E9-C00C-4BA8-8E4B-ABBBEC3A62B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14040" firstSheet="4" activeTab="4" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="13905" firstSheet="4" activeTab="4" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
   </bookViews>
   <sheets>
     <sheet name="General Errors" sheetId="9" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3758" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3798" uniqueCount="958">
   <si>
     <t>API</t>
   </si>
@@ -2910,12 +2910,48 @@
   <si>
     <t>RECTANGLE' is only supported for Return Labels with 'imageInfo.labelType' of '4X5LABEL'</t>
   </si>
+  <si>
+    <t>https://api.usps.com/labels/v3/indicia/imb/{imb#}</t>
+  </si>
+  <si>
+    <t>packageOptions.originalPackage.originalTrackingNumber is currently not supported when packageOptions.returnReceiptTracking is true</t>
+  </si>
+  <si>
+    <t>Indicia not found.</t>
+  </si>
+  <si>
+    <t>letter/flat cannot be more than %d days in the past</t>
+  </si>
+  <si>
+    <t>letter/flat is already canceled</t>
+  </si>
+  <si>
+    <t>letter/flat is already disputed</t>
+  </si>
+  <si>
+    <t>Forbidden</t>
+  </si>
+  <si>
+    <t>4X4LABEL currently does not support imageInfo.imageType of 'ZPL203DPI' or 'ZPL300DPI'</t>
+  </si>
+  <si>
+    <t>packageOptions.returnReceiptTracking</t>
+  </si>
+  <si>
+    <t>imb</t>
+  </si>
+  <si>
+    <t>imb.mailingDate</t>
+  </si>
+  <si>
+    <t>imb.status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2993,6 +3029,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3020,7 +3061,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3148,6 +3189,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -7411,11 +7456,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G209"/>
+  <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D198" sqref="D198"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D219" sqref="D219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12226,6 +12271,167 @@
         <v>945</v>
       </c>
     </row>
+    <row r="210" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B210" s="20">
+        <v>400</v>
+      </c>
+      <c r="C210" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D210" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E210" s="17">
+        <v>160360</v>
+      </c>
+      <c r="F210" s="37" t="s">
+        <v>954</v>
+      </c>
+      <c r="G210" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B211" s="20">
+        <v>400</v>
+      </c>
+      <c r="C211" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D211" s="45" t="s">
+        <v>946</v>
+      </c>
+      <c r="E211" s="17">
+        <v>160361</v>
+      </c>
+      <c r="F211" s="17" t="s">
+        <v>955</v>
+      </c>
+      <c r="G211" s="2" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B212" s="20">
+        <v>400</v>
+      </c>
+      <c r="C212" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D212" s="45" t="s">
+        <v>946</v>
+      </c>
+      <c r="E212" s="17">
+        <v>160362</v>
+      </c>
+      <c r="F212" s="17" t="s">
+        <v>956</v>
+      </c>
+      <c r="G212" s="2" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B213" s="20">
+        <v>400</v>
+      </c>
+      <c r="C213" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D213" s="45" t="s">
+        <v>946</v>
+      </c>
+      <c r="E213" s="17">
+        <v>160363</v>
+      </c>
+      <c r="F213" s="17" t="s">
+        <v>957</v>
+      </c>
+      <c r="G213" s="2" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B214" s="20">
+        <v>400</v>
+      </c>
+      <c r="C214" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D214" s="45" t="s">
+        <v>946</v>
+      </c>
+      <c r="E214" s="17">
+        <v>160364</v>
+      </c>
+      <c r="F214" s="17" t="s">
+        <v>957</v>
+      </c>
+      <c r="G214" s="2" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B215" s="20">
+        <v>400</v>
+      </c>
+      <c r="C215" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D215" s="45" t="s">
+        <v>946</v>
+      </c>
+      <c r="E215" s="17">
+        <v>160364</v>
+      </c>
+      <c r="F215" s="17" t="s">
+        <v>955</v>
+      </c>
+      <c r="G215" s="2" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B216" s="20">
+        <v>400</v>
+      </c>
+      <c r="C216" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D216" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E216" s="17">
+        <v>160366</v>
+      </c>
+      <c r="F216" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="G216" s="46" t="s">
+        <v>953</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{A36F69E6-5AC8-443F-8567-4E3FB7E927F1}"/>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -12239,10 +12445,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView topLeftCell="D171" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183:G186"/>
+    <sheetView topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="D193" sqref="D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16356,8 +16562,8 @@
       </c>
     </row>
     <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" s="21" t="s">
-        <v>91</v>
+      <c r="A181" s="10" t="s">
+        <v>375</v>
       </c>
       <c r="B181" s="21">
         <v>400</v>
@@ -16379,8 +16585,8 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A182" s="21" t="s">
-        <v>91</v>
+      <c r="A182" s="10" t="s">
+        <v>375</v>
       </c>
       <c r="B182" s="21">
         <v>400</v>
@@ -16402,8 +16608,8 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" s="21" t="s">
-        <v>91</v>
+      <c r="A183" s="10" t="s">
+        <v>375</v>
       </c>
       <c r="B183" s="21">
         <v>400</v>
@@ -16425,8 +16631,8 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="21" t="s">
-        <v>91</v>
+      <c r="A184" s="10" t="s">
+        <v>375</v>
       </c>
       <c r="B184" s="21">
         <v>400</v>
@@ -16448,8 +16654,8 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" s="21" t="s">
-        <v>91</v>
+      <c r="A185" s="10" t="s">
+        <v>375</v>
       </c>
       <c r="B185" s="21">
         <v>400</v>
@@ -16471,8 +16677,8 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A186" s="21" t="s">
-        <v>91</v>
+      <c r="A186" s="10" t="s">
+        <v>375</v>
       </c>
       <c r="B186" s="21">
         <v>400</v>
@@ -16491,6 +16697,29 @@
       </c>
       <c r="G186" t="s">
         <v>945</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B187" s="21">
+        <v>400</v>
+      </c>
+      <c r="C187" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D187" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E187" s="17">
+        <v>160366</v>
+      </c>
+      <c r="F187" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="G187" s="46" t="s">
+        <v>953</v>
       </c>
     </row>
   </sheetData>
@@ -18935,6 +19164,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -18945,15 +19183,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19203,6 +19432,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DC8D4E-C199-4BF9-AF5D-F16C7D7041E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -19216,14 +19453,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
New Updated error file for 7/11
Error list update for 7/11
</commit_message>
<xml_diff>
--- a/Error Inventory/API Error Consolidated List.xlsx
+++ b/Error Inventory/API Error Consolidated List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eagnmnwbp130a.usa.dce.usps.gov\VDIProfiles$\fsbtg0\Documents\API Consolidated file to upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51CC7E9-C00C-4BA8-8E4B-ABBBEC3A62B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0EEB95-4D90-400C-842B-94B44D0E0F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="13905" firstSheet="4" activeTab="4" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13920" activeTab="5" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
   </bookViews>
   <sheets>
     <sheet name="General Errors" sheetId="9" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3798" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="971">
   <si>
     <t>API</t>
   </si>
@@ -2946,12 +2946,51 @@
   <si>
     <t>imb.status</t>
   </si>
+  <si>
+    <t>6X4LABEL is not currently supported</t>
+  </si>
+  <si>
+    <t>imageInfo.imageType, imageInfo.labelType, imageInfo.receiptOption</t>
+  </si>
+  <si>
+    <t>Label Broker Service is unavailable. For any questions, please reach out to us at https://emailus.usps.com/s/web-tools-inquiry</t>
+  </si>
+  <si>
+    <t>PAYER role required</t>
+  </si>
+  <si>
+    <t>&lt;labelType&gt; currently does not support imageInfo.imageType of 'ZPL203DPI' or 'ZPL300DPI' with imageInfo.receiptOption of 'SEPARATE_PAGE'</t>
+  </si>
+  <si>
+    <t>ESC 915 or 917 may not be used for articles sent to or from &lt;location&gt;</t>
+  </si>
+  <si>
+    <t>impbContainerType, containerMailClass</t>
+  </si>
+  <si>
+    <t>impbContainerType, imcbContainerType</t>
+  </si>
+  <si>
+    <t>OPEN_DISTRIBUTE_PALLET container type is only supported for PRIORITY_MAIL mail class</t>
+  </si>
+  <si>
+    <t>must be less than or equal to 70.0</t>
+  </si>
+  <si>
+    <t>Containers with containerMailClass PRIORITY_MAIL and imcbContainerType/impbContainerType SACK cannot contain HAZMAT packages</t>
+  </si>
+  <si>
+    <t>160372</t>
+  </si>
+  <si>
+    <t>LABEL_PROVIDER only supports the accountType of EPS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3034,6 +3073,20 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3057,9 +3110,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3191,13 +3245,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3915,10 +3972,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4322,6 +4379,29 @@
         <v>688</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>558</v>
+      </c>
+      <c r="B18">
+        <v>400</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>562</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>969</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>826</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>970</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4332,10 +4412,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4434,7 +4514,7 @@
       <c r="E4" s="17">
         <v>160321</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="17" t="s">
         <v>876</v>
       </c>
       <c r="G4" t="s">
@@ -4457,7 +4537,7 @@
       <c r="E5" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="24" t="s">
         <v>830</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -4480,7 +4560,7 @@
       <c r="E6" s="17">
         <v>160344</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="17" t="s">
         <v>939</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -4503,7 +4583,7 @@
       <c r="E7" s="17">
         <v>160345</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="17" t="s">
         <v>939</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -4526,7 +4606,7 @@
       <c r="E8" s="17">
         <v>160350</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="17" t="s">
         <v>938</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -4549,7 +4629,7 @@
       <c r="E9" s="17">
         <v>160352</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="17" t="s">
         <v>938</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -4572,7 +4652,7 @@
       <c r="E10" s="17">
         <v>160353</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="17" t="s">
         <v>938</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -4595,7 +4675,7 @@
       <c r="E11" s="17">
         <v>160354</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="17" t="s">
         <v>938</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -4618,11 +4698,80 @@
       <c r="E12" s="17">
         <v>160355</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="17" t="s">
         <v>938</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>937</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B13" s="10">
+        <v>400</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E13" s="17">
+        <v>160371</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>964</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B14" s="10">
+        <v>400</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E14" s="17">
+        <v>160373</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>788</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="B15" s="10">
+        <v>400</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E15" s="17">
+        <v>160374</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>965</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>968</v>
       </c>
     </row>
   </sheetData>
@@ -7456,11 +7605,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G216"/>
+  <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D219" sqref="D219"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F221" sqref="F221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12304,7 +12453,7 @@
       <c r="C211" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D211" s="45" t="s">
+      <c r="D211" t="s">
         <v>946</v>
       </c>
       <c r="E211" s="17">
@@ -12327,7 +12476,7 @@
       <c r="C212" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D212" s="45" t="s">
+      <c r="D212" t="s">
         <v>946</v>
       </c>
       <c r="E212" s="17">
@@ -12350,7 +12499,7 @@
       <c r="C213" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D213" s="45" t="s">
+      <c r="D213" t="s">
         <v>946</v>
       </c>
       <c r="E213" s="17">
@@ -12373,7 +12522,7 @@
       <c r="C214" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D214" s="45" t="s">
+      <c r="D214" t="s">
         <v>946</v>
       </c>
       <c r="E214" s="17">
@@ -12396,7 +12545,7 @@
       <c r="C215" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D215" s="45" t="s">
+      <c r="D215" t="s">
         <v>946</v>
       </c>
       <c r="E215" s="17">
@@ -12428,8 +12577,123 @@
       <c r="F216" s="17" t="s">
         <v>715</v>
       </c>
-      <c r="G216" s="46" t="s">
+      <c r="G216" s="45" t="s">
         <v>953</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A217" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B217" s="20">
+        <v>400</v>
+      </c>
+      <c r="C217" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D217" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E217" s="17">
+        <v>160367</v>
+      </c>
+      <c r="F217" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="G217" s="2" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B218" s="20">
+        <v>400</v>
+      </c>
+      <c r="C218" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D218" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E218" s="17">
+        <v>160368</v>
+      </c>
+      <c r="F218" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="G218" s="2" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B219" s="20">
+        <v>400</v>
+      </c>
+      <c r="C219" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D219" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E219" s="17">
+        <v>160369</v>
+      </c>
+      <c r="F219" s="17" t="s">
+        <v>800</v>
+      </c>
+      <c r="G219" s="2" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A220" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B220" s="21">
+        <v>400</v>
+      </c>
+      <c r="C220" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D220" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E220" s="24">
+        <v>160370</v>
+      </c>
+      <c r="F220" s="33" t="s">
+        <v>959</v>
+      </c>
+      <c r="G220" s="11" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B221" s="20">
+        <v>400</v>
+      </c>
+      <c r="C221" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D221" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E221" s="17">
+        <v>160375</v>
+      </c>
+      <c r="F221" s="17" t="s">
+        <v>733</v>
+      </c>
+      <c r="G221" s="2" t="s">
+        <v>963</v>
       </c>
     </row>
   </sheetData>
@@ -12445,10 +12709,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G187"/>
+  <dimension ref="A1:G190"/>
   <sheetViews>
-    <sheetView topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="D193" sqref="D193"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16718,8 +16982,77 @@
       <c r="F187" s="17" t="s">
         <v>715</v>
       </c>
-      <c r="G187" s="46" t="s">
+      <c r="G187" s="45" t="s">
         <v>953</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B188" s="21">
+        <v>400</v>
+      </c>
+      <c r="C188" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D188" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E188" s="17">
+        <v>160367</v>
+      </c>
+      <c r="F188" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="G188" s="2" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A189" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B189" s="21">
+        <v>400</v>
+      </c>
+      <c r="C189" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D189" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E189" s="24">
+        <v>160368</v>
+      </c>
+      <c r="F189" s="24" t="s">
+        <v>716</v>
+      </c>
+      <c r="G189" s="11" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A190" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B190" s="21">
+        <v>400</v>
+      </c>
+      <c r="C190" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D190" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E190" s="24">
+        <v>160370</v>
+      </c>
+      <c r="F190" s="33" t="s">
+        <v>959</v>
+      </c>
+      <c r="G190" s="11" t="s">
+        <v>962</v>
       </c>
     </row>
   </sheetData>
@@ -19164,28 +19497,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD1EFD7F07544F4C8A5DF6ACE5557D0F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0a46465e297c47d8b88a71685f887e65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9" xmlns:ns3="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4503a5f252426d71f93d44927b16e869" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19431,10 +19742,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11AB0D6-FBA0-4F11-8778-05A9ADBB93A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
+    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19458,21 +19803,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F11AB0D6-FBA0-4F11-8778-05A9ADBB93A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
-    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Error List File - 10/30/2025
</commit_message>
<xml_diff>
--- a/Error Inventory/API Error Consolidated List.xlsx
+++ b/Error Inventory/API Error Consolidated List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eagnmnwbp130a.usa.dce.usps.gov\VDIProfiles$\fsbtg0\Documents\API Consolidated file to upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F448109-556B-48A9-BBCE-95366CD8D1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221AFA77-C70C-4A96-B5FD-8FDE26F499FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="13785" firstSheet="3" activeTab="4" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13920" firstSheet="11" activeTab="12" xr2:uid="{BD4CA92B-BD2B-408A-B66B-5389FE5197CE}"/>
   </bookViews>
   <sheets>
     <sheet name="General Errors" sheetId="9" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4000" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4010" uniqueCount="1009">
   <si>
     <t>API</t>
   </si>
@@ -3112,6 +3112,12 @@
   </si>
   <si>
     <t>at least 1 item is required when requesting duties, taxes, and fees</t>
+  </si>
+  <si>
+    <t>barcode &lt;barcode&gt; has been canceled and is not eligible to be added to a SCAN Form</t>
+  </si>
+  <si>
+    <t>barcode&lt;barcode &gt;has manifested and is not eligible to be added to a SCAN Form</t>
   </si>
 </sst>
 </file>
@@ -3255,7 +3261,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3392,7 +3398,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4012,7 +4017,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60">
+    <row r="7" spans="1:7" ht="45">
       <c r="A7" s="10" t="s">
         <v>524</v>
       </c>
@@ -4035,7 +4040,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60">
+    <row r="8" spans="1:7" ht="45">
       <c r="A8" s="10" t="s">
         <v>524</v>
       </c>
@@ -5179,10 +5184,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5539,7 +5544,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7">
       <c r="A16" s="10" t="s">
         <v>572</v>
       </c>
@@ -5560,6 +5565,52 @@
       </c>
       <c r="G16" t="s">
         <v>602</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="B17" s="10">
+        <v>400</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>979</v>
+      </c>
+      <c r="E17" s="24">
+        <v>160397</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>756</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="B18" s="10">
+        <v>400</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>979</v>
+      </c>
+      <c r="E18" s="24">
+        <v>160398</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>756</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>1008</v>
       </c>
     </row>
   </sheetData>
@@ -8048,8 +8099,8 @@
   </sheetPr>
   <dimension ref="A1:G232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F234" sqref="F234"/>
     </sheetView>
   </sheetViews>
@@ -13354,7 +13405,7 @@
       <c r="C231" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D231" s="48" t="s">
+      <c r="D231" t="s">
         <v>1004</v>
       </c>
       <c r="E231" s="17">
@@ -17787,7 +17838,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -17826,7 +17877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="11" customFormat="1">
+    <row r="2" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A2" s="10" t="s">
         <v>415</v>
       </c>
@@ -17847,7 +17898,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="11" customFormat="1">
+    <row r="3" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A3" s="11" t="s">
         <v>415</v>
       </c>
@@ -17893,7 +17944,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="10" t="s">
         <v>415</v>
       </c>
@@ -17916,7 +17967,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="10" t="s">
         <v>415</v>
       </c>
@@ -17939,7 +17990,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="10" t="s">
         <v>415</v>
       </c>
@@ -17962,7 +18013,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="10" t="s">
         <v>415</v>
       </c>
@@ -17985,7 +18036,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="10" t="s">
         <v>415</v>
       </c>
@@ -18029,7 +18080,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="10" t="s">
         <v>415</v>
       </c>
@@ -18052,7 +18103,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="10" t="s">
         <v>415</v>
       </c>
@@ -18073,7 +18124,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="10" t="s">
         <v>415</v>
       </c>
@@ -18094,7 +18145,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="30">
       <c r="A14" s="10" t="s">
         <v>415</v>
       </c>
@@ -18157,7 +18208,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="30">
       <c r="A17" s="10" t="s">
         <v>415</v>
       </c>
@@ -18180,7 +18231,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="30">
       <c r="A18" s="10" t="s">
         <v>415</v>
       </c>
@@ -18203,7 +18254,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="30">
       <c r="A19" s="10" t="s">
         <v>415</v>
       </c>
@@ -18226,7 +18277,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="30">
       <c r="A20" s="10" t="s">
         <v>415</v>
       </c>
@@ -18249,7 +18300,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="30">
       <c r="A21" s="10" t="s">
         <v>415</v>
       </c>
@@ -18272,7 +18323,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="30">
       <c r="A22" s="10" t="s">
         <v>415</v>
       </c>
@@ -18295,7 +18346,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="30">
       <c r="A23" s="10" t="s">
         <v>415</v>
       </c>
@@ -18316,7 +18367,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="30">
       <c r="A24" s="10" t="s">
         <v>415</v>
       </c>
@@ -18337,7 +18388,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="30">
       <c r="A25" s="10" t="s">
         <v>415</v>
       </c>
@@ -18358,7 +18409,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="30">
       <c r="A26" s="10" t="s">
         <v>415</v>
       </c>
@@ -18381,7 +18432,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="60">
       <c r="A27" s="10" t="s">
         <v>415</v>
       </c>
@@ -18801,7 +18852,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>475</v>
       </c>
@@ -18958,7 +19009,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" t="s">
         <v>475</v>
       </c>
@@ -19567,8 +19618,8 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19652,7 +19703,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="11" t="s">
         <v>521</v>
       </c>
@@ -19675,7 +19726,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="11" t="s">
         <v>521</v>
       </c>
@@ -19698,7 +19749,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="11" t="s">
         <v>521</v>
       </c>
@@ -19721,7 +19772,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="11" t="s">
         <v>521</v>
       </c>
@@ -19744,7 +19795,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="11" t="s">
         <v>521</v>
       </c>
@@ -19788,7 +19839,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="30">
       <c r="A10" s="11" t="s">
         <v>521</v>
       </c>
@@ -19811,7 +19862,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="11" customFormat="1">
+    <row r="11" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A11" s="11" t="s">
         <v>521</v>
       </c>
@@ -19832,7 +19883,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="11" customFormat="1">
+    <row r="12" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A12" s="11" t="s">
         <v>521</v>
       </c>
@@ -19853,7 +19904,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="11" customFormat="1">
+    <row r="13" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A13" s="11" t="s">
         <v>521</v>
       </c>
@@ -19895,7 +19946,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="11" customFormat="1">
+    <row r="15" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A15" s="11" t="s">
         <v>521</v>
       </c>
@@ -19916,7 +19967,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="11" customFormat="1">
+    <row r="16" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A16" s="11" t="s">
         <v>521</v>
       </c>
@@ -19937,7 +19988,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="11" customFormat="1">
+    <row r="17" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A17" s="11" t="s">
         <v>521</v>
       </c>
@@ -19958,7 +20009,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="11" customFormat="1">
+    <row r="18" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A18" s="11" t="s">
         <v>521</v>
       </c>
@@ -19979,7 +20030,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="11" customFormat="1">
+    <row r="19" spans="1:7" s="11" customFormat="1" ht="30">
       <c r="A19" s="11" t="s">
         <v>521</v>
       </c>
@@ -20002,7 +20053,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30">
+    <row r="20" spans="1:7" ht="60">
       <c r="A20" s="11" t="s">
         <v>521</v>
       </c>
@@ -20048,7 +20099,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="30">
       <c r="A22" s="11" t="s">
         <v>521</v>
       </c>
@@ -20071,7 +20122,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="30">
       <c r="A23" s="11" t="s">
         <v>521</v>
       </c>
@@ -20094,7 +20145,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="30">
       <c r="A24" s="11" t="s">
         <v>521</v>
       </c>
@@ -20245,7 +20296,7 @@
       <c r="D30" s="11" t="s">
         <v>973</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="24">
         <v>160396</v>
       </c>
       <c r="F30" s="17" t="s">
@@ -20262,16 +20313,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20521,28 +20568,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DC8D4E-C199-4BF9-AF5D-F16C7D7041E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20568,9 +20609,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D590CCA9-7961-4660-BBC6-10104A0DDFD4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DC8D4E-C199-4BF9-AF5D-F16C7D7041E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2595f96f-d2aa-4fa4-b5ed-10baae53ecb9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9cf85ca5-4acf-45da-adaa-d6bfc34b6c9f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>